<commit_message>
Actualizacion de menu vertical y otros de filtrado
</commit_message>
<xml_diff>
--- a/uploads/Cantidades/Cantidad Panulcillo.xlsx
+++ b/uploads/Cantidades/Cantidad Panulcillo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enami-my.sharepoint.com/personal/pjdiaz_enami_cl/Documents/Escritorio/Proyecto37/Proyecto16/Proyecto11/proyecto2/uploads/Cantidades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_AD4D2F04E46CFB4ACB3E20C07D90DEBA683EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{523085D1-03EB-4AF0-B067-0ADA0181D0D5}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="11_AD4D2F04E46CFB4ACB3E20C07D90DEBA683EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50F17E26-B9F7-4D42-B81D-1FD82262C2FE}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="19">
   <si>
     <t>id_categoria</t>
   </si>
@@ -43,6 +43,45 @@
   </si>
   <si>
     <t>HH</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>un</t>
+  </si>
+  <si>
+    <t>VIAJE</t>
   </si>
 </sst>
 </file>
@@ -416,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -807,6 +846,538 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>44101</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <v>63561</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="4">
+        <v>44102</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>359053</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>44103</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="4">
+        <v>44104</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="3">
+        <v>44105</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="4">
+        <v>44106</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>1786</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="3">
+        <v>44107</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>280</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="4">
+        <v>44108</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="3">
+        <v>44109</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>956</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="4">
+        <v>44110</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <v>919</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="3">
+        <v>44111</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>2434</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="4">
+        <v>44112</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>2757</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="3">
+        <v>44113</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>63</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="4">
+        <v>44114</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41">
+        <v>46</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="3">
+        <v>44115</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42">
+        <v>1344</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="4">
+        <v>44116</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43">
+        <v>26797</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="3">
+        <v>44117</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <v>3432</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="4">
+        <v>44118</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>799</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="3">
+        <v>44119</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>96</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="4">
+        <v>44120</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47">
+        <v>3432</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="3">
+        <v>44121</v>
+      </c>
+      <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48">
+        <v>3119</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="4">
+        <v>44122</v>
+      </c>
+      <c r="B49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49">
+        <v>347</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="3">
+        <v>44123</v>
+      </c>
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50">
+        <v>1021</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="4">
+        <v>44124</v>
+      </c>
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51">
+        <v>1021</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="3">
+        <v>44125</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="4">
+        <v>44126</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>1097</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="3">
+        <v>44127</v>
+      </c>
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54">
+        <v>848</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="4">
+        <v>44128</v>
+      </c>
+      <c r="B55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55">
+        <v>52</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="3">
+        <v>44129</v>
+      </c>
+      <c r="B56" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56">
+        <v>12</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="4">
+        <v>44130</v>
+      </c>
+      <c r="B57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57">
+        <v>12</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="3">
+        <v>44131</v>
+      </c>
+      <c r="B58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58">
+        <v>1184</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="4">
+        <v>44132</v>
+      </c>
+      <c r="B59" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59">
+        <v>46</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="3">
+        <v>44133</v>
+      </c>
+      <c r="B60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60">
+        <v>442</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="4">
+        <v>44134</v>
+      </c>
+      <c r="B61" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61">
+        <v>89</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="3">
+        <v>44135</v>
+      </c>
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62">
+        <v>104</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="4">
+        <v>44136</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63">
+        <v>1736</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="3">
+        <v>44137</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64">
+        <v>158</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="4">
+        <v>44138</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>